<commit_message>
brought to working condition
</commit_message>
<xml_diff>
--- a/backend/excel_to_databases/all_blogposts.xlsx
+++ b/backend/excel_to_databases/all_blogposts.xlsx
@@ -7,9 +7,10 @@
   <sheets>
     <sheet name="all_blogposts" sheetId="1" r:id="rId1"/>
     <sheet name="comments" sheetId="2" r:id="rId2"/>
-    <sheet name="users" sheetId="3" r:id="rId3"/>
-    <sheet name="sheets_classes" sheetId="4" r:id="rId4"/>
-    <sheet name="relationship_structure" sheetId="5" r:id="rId5"/>
+    <sheet name="likes" sheetId="3" r:id="rId3"/>
+    <sheet name="users" sheetId="4" r:id="rId4"/>
+    <sheet name="sheets_classes" sheetId="5" r:id="rId5"/>
+    <sheet name="relationship_structure" sheetId="6" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
@@ -23,6 +24,9 @@
     <t>comments</t>
   </si>
   <si>
+    <t>likes</t>
+  </si>
+  <si>
     <t>users</t>
   </si>
   <si>
@@ -32,6 +36,9 @@
     <t>Comment</t>
   </si>
   <si>
+    <t>Like</t>
+  </si>
+  <si>
     <t>User</t>
   </si>
   <si>
@@ -50,24 +57,15 @@
     <t>date_of_publishing</t>
   </si>
   <si>
-    <t>author_name</t>
+    <t>initial_tags</t>
+  </si>
+  <si>
+    <t>endpoint</t>
   </si>
   <si>
     <t>first_para</t>
   </si>
   <si>
-    <t>total_likes</t>
-  </si>
-  <si>
-    <t>total_shares</t>
-  </si>
-  <si>
-    <t>endpoint</t>
-  </si>
-  <si>
-    <t>initial_tags</t>
-  </si>
-  <si>
     <t>second_para</t>
   </si>
   <si>
@@ -83,9 +81,6 @@
     <t>all_tags</t>
   </si>
   <si>
-    <t>author_details</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
@@ -125,28 +120,16 @@
     <t>12</t>
   </si>
   <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
     <t>reference_for_all_blogposts</t>
   </si>
   <si>
-    <t>image_thumbnail</t>
-  </si>
-  <si>
     <t>text</t>
   </si>
   <si>
-    <t>comment_order</t>
+    <t>commenting_timestamp</t>
+  </si>
+  <si>
+    <t>timestamp_of_liking</t>
   </si>
   <si>
     <t>user_name</t>
@@ -155,6 +138,15 @@
     <t>phone_number</t>
   </si>
   <si>
+    <t>user_image</t>
+  </si>
+  <si>
+    <t>hash</t>
+  </si>
+  <si>
+    <t>salt</t>
+  </si>
+  <si>
     <t>parent</t>
   </si>
   <si>
@@ -173,13 +165,22 @@
     <t>child2_range</t>
   </si>
   <si>
-    <t>1,17</t>
+    <t>child3</t>
+  </si>
+  <si>
+    <t>child3_range</t>
+  </si>
+  <si>
+    <t>1,13</t>
+  </si>
+  <si>
+    <t>1,3</t>
+  </si>
+  <si>
+    <t>1,2</t>
   </si>
   <si>
     <t>1,6</t>
-  </si>
-  <si>
-    <t>1,3</t>
   </si>
 </sst>
 </file>
@@ -223,116 +224,92 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17">
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O2" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -341,6 +318,70 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -350,42 +391,42 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -393,34 +434,40 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>45</v>
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -428,86 +475,63 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>